<commit_message>
Added some texts for Concepts.
</commit_message>
<xml_diff>
--- a/Bewertungsmatrixnew.xlsx
+++ b/Bewertungsmatrixnew.xlsx
@@ -1,26 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="26709"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/heuby/Library/Mobile Documents/com~apple~CloudDocs/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2100" yWindow="6120" windowWidth="24760" windowHeight="16440"/>
+    <workbookView xWindow="2100" yWindow="6120" windowWidth="24765" windowHeight="16440"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -28,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="63">
   <si>
     <t>Nr</t>
   </si>
@@ -129,9 +124,6 @@
     <t>Datenspeicherung</t>
   </si>
   <si>
-    <t>Deployment Pipeline</t>
-  </si>
-  <si>
     <t>Schnittstellen Versionierung</t>
   </si>
   <si>
@@ -150,9 +142,6 @@
     <t>Key-Value Redis</t>
   </si>
   <si>
-    <t>Column1</t>
-  </si>
-  <si>
     <t>Document MongoDB</t>
   </si>
   <si>
@@ -202,15 +191,6 @@
   </si>
   <si>
     <t>Interportabilität</t>
-  </si>
-  <si>
-    <t>Column2</t>
-  </si>
-  <si>
-    <t>Column3</t>
-  </si>
-  <si>
-    <t>Column4</t>
   </si>
   <si>
     <t>Strategisch</t>
@@ -616,7 +596,7 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -673,39 +653,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="14" xfId="4" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="15" xfId="4" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="16" xfId="4" applyFont="1" applyBorder="1"/>
@@ -736,6 +683,42 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="24" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="14" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="15" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="16" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Currency" xfId="3" builtinId="4"/>
@@ -744,79 +727,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Output" xfId="4" builtinId="21"/>
   </cellStyles>
-  <dxfs count="42">
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color theme="1" tint="0.34998626667073579"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color theme="1" tint="0.34998626667073579"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
+  <dxfs count="34">
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1116,30 +1027,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:V17" totalsRowShown="0">
-  <tableColumns count="22">
-    <tableColumn id="1" name="Nr" dataDxfId="41"/>
-    <tableColumn id="2" name="Beschreibung" dataDxfId="40" totalsRowDxfId="39"/>
-    <tableColumn id="12" name="Gewicht" dataDxfId="38" totalsRowDxfId="37"/>
-    <tableColumn id="7" name="RDBMS Oracle" totalsRowDxfId="36"/>
-    <tableColumn id="5" name="RDBMS MySQL" dataDxfId="35" totalsRowDxfId="34"/>
-    <tableColumn id="6" name="Key-Value Redis" dataDxfId="33" totalsRowDxfId="32"/>
-    <tableColumn id="8" name="Document MongoDB" dataDxfId="31" totalsRowDxfId="30"/>
-    <tableColumn id="11" name="Pfad" dataDxfId="29" totalsRowDxfId="28"/>
-    <tableColumn id="10" name="Content-Negotiation" dataDxfId="27" totalsRowDxfId="26"/>
-    <tableColumn id="3" name="GraphQL" dataDxfId="25" totalsRowDxfId="24"/>
-    <tableColumn id="20" name="Message-Queue JMS" dataDxfId="23" totalsRowDxfId="22"/>
-    <tableColumn id="19" name="Message-Queue Kafka" dataDxfId="21" totalsRowDxfId="20"/>
-    <tableColumn id="18" name="Mesage-Queue Redis" dataDxfId="19" totalsRowDxfId="18"/>
-    <tableColumn id="25" name="Spring-Rest" dataDxfId="17" totalsRowDxfId="16"/>
-    <tableColumn id="24" name="Docker Compose,Swarm" dataDxfId="15" totalsRowDxfId="14"/>
-    <tableColumn id="23" name="Kubernetes" dataDxfId="13" totalsRowDxfId="12"/>
-    <tableColumn id="22" name="SaltStack" dataDxfId="11" totalsRowDxfId="10"/>
-    <tableColumn id="26" name="Spring Cloud Config" dataDxfId="9" totalsRowDxfId="8"/>
-    <tableColumn id="28" name="Column1" dataDxfId="7" totalsRowDxfId="6"/>
-    <tableColumn id="27" name="Column2" dataDxfId="5" totalsRowDxfId="4"/>
-    <tableColumn id="29" name="Column3" dataDxfId="3" totalsRowDxfId="2"/>
-    <tableColumn id="9" name="Column4" dataDxfId="1" totalsRowDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:R17" totalsRowShown="0">
+  <tableColumns count="18">
+    <tableColumn id="1" name="Nr" dataDxfId="33"/>
+    <tableColumn id="2" name="Beschreibung" dataDxfId="32" totalsRowDxfId="31"/>
+    <tableColumn id="12" name="Gewicht" dataDxfId="30" totalsRowDxfId="29"/>
+    <tableColumn id="7" name="RDBMS Oracle" totalsRowDxfId="28"/>
+    <tableColumn id="5" name="RDBMS MySQL" dataDxfId="27" totalsRowDxfId="26"/>
+    <tableColumn id="6" name="Key-Value Redis" dataDxfId="25" totalsRowDxfId="24"/>
+    <tableColumn id="8" name="Document MongoDB" dataDxfId="23" totalsRowDxfId="22"/>
+    <tableColumn id="11" name="Pfad" dataDxfId="21" totalsRowDxfId="20"/>
+    <tableColumn id="10" name="Content-Negotiation" dataDxfId="19" totalsRowDxfId="18"/>
+    <tableColumn id="3" name="GraphQL" dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="20" name="Message-Queue JMS" dataDxfId="15" totalsRowDxfId="14"/>
+    <tableColumn id="19" name="Message-Queue Kafka" dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="18" name="Mesage-Queue Redis" dataDxfId="11" totalsRowDxfId="10"/>
+    <tableColumn id="25" name="Spring-Rest" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="24" name="Docker Compose,Swarm" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="23" name="Kubernetes" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="22" name="SaltStack" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="26" name="Spring Cloud Config" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1434,7 +1341,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1442,81 +1349,71 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V35"/>
+  <dimension ref="A1:R35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:V19"/>
+      <selection activeCell="X3" sqref="X3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.33203125" customWidth="1"/>
-    <col min="2" max="2" width="45.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="22" width="4.5" customWidth="1"/>
+    <col min="1" max="1" width="6.28515625" customWidth="1"/>
+    <col min="2" max="2" width="45.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="18" width="4.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:18" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23"/>
-      <c r="O1" s="23"/>
-      <c r="P1" s="23"/>
-      <c r="Q1" s="23"/>
-      <c r="R1" s="23"/>
-      <c r="S1" s="23"/>
-      <c r="T1" s="23"/>
-      <c r="U1" s="23"/>
-      <c r="V1" s="23"/>
-    </row>
-    <row r="2" spans="1:22" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="30"/>
-      <c r="B2" s="30"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="24" t="s">
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="38"/>
+      <c r="Q1" s="38"/>
+      <c r="R1" s="38"/>
+    </row>
+    <row r="2" spans="1:18" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="45"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="24" t="s">
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="24" t="s">
+      <c r="L2" s="40"/>
+      <c r="M2" s="40"/>
+      <c r="N2" s="41"/>
+      <c r="O2" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="L2" s="25"/>
-      <c r="M2" s="25"/>
-      <c r="N2" s="26"/>
-      <c r="O2" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="P2" s="28"/>
-      <c r="Q2" s="28"/>
-      <c r="R2" s="29"/>
-      <c r="S2" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="T2" s="28"/>
-      <c r="U2" s="28"/>
-      <c r="V2" s="29"/>
-    </row>
-    <row r="3" spans="1:22" ht="133" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P2" s="43"/>
+      <c r="Q2" s="43"/>
+      <c r="R2" s="44"/>
+    </row>
+    <row r="3" spans="1:18" ht="132.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
@@ -1527,69 +1424,57 @@
         <v>19</v>
       </c>
       <c r="D3" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="F3" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="18" t="s">
+      <c r="G3" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="G3" s="19" t="s">
+      <c r="H3" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="I3" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="J3" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="I3" s="18" t="s">
+      <c r="K3" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="J3" s="18" t="s">
+      <c r="L3" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="K3" s="17" t="s">
+      <c r="M3" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="L3" s="18" t="s">
+      <c r="N3" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="M3" s="18" t="s">
+      <c r="O3" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="N3" s="19" t="s">
+      <c r="P3" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="O3" s="17" t="s">
+      <c r="Q3" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="P3" s="18" t="s">
+      <c r="R3" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="Q3" s="18" t="s">
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="R3" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="S3" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="T3" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="U3" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="V3" s="19" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>53</v>
       </c>
       <c r="C4" s="2">
         <v>5</v>
@@ -1633,17 +1518,13 @@
       <c r="R4" s="8">
         <v>4</v>
       </c>
-      <c r="S4" s="7"/>
-      <c r="T4" s="4"/>
-      <c r="U4" s="5"/>
-      <c r="V4" s="8"/>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C5" s="2">
         <v>4</v>
@@ -1693,12 +1574,8 @@
       <c r="R5" s="8">
         <v>4</v>
       </c>
-      <c r="S5" s="7"/>
-      <c r="T5" s="4"/>
-      <c r="U5" s="5"/>
-      <c r="V5" s="8"/>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>7</v>
       </c>
@@ -1731,12 +1608,8 @@
       <c r="P6" s="4"/>
       <c r="Q6" s="5"/>
       <c r="R6" s="8"/>
-      <c r="S6" s="7"/>
-      <c r="T6" s="4"/>
-      <c r="U6" s="5"/>
-      <c r="V6" s="8"/>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>8</v>
       </c>
@@ -1791,17 +1664,13 @@
       <c r="R7" s="8">
         <v>5</v>
       </c>
-      <c r="S7" s="7"/>
-      <c r="T7" s="4"/>
-      <c r="U7" s="5"/>
-      <c r="V7" s="8"/>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C8" s="2">
         <v>3</v>
@@ -1851,17 +1720,13 @@
       <c r="R8" s="8">
         <v>4</v>
       </c>
-      <c r="S8" s="7"/>
-      <c r="T8" s="4"/>
-      <c r="U8" s="5"/>
-      <c r="V8" s="8"/>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C9" s="2">
         <v>3</v>
@@ -1911,12 +1776,8 @@
       <c r="R9" s="8">
         <v>5</v>
       </c>
-      <c r="S9" s="7"/>
-      <c r="T9" s="4"/>
-      <c r="U9" s="5"/>
-      <c r="V9" s="8"/>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>11</v>
       </c>
@@ -1971,17 +1832,13 @@
       <c r="R10" s="8">
         <v>5</v>
       </c>
-      <c r="S10" s="7"/>
-      <c r="T10" s="4"/>
-      <c r="U10" s="5"/>
-      <c r="V10" s="8"/>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C11" s="2">
         <v>3</v>
@@ -2001,12 +1858,8 @@
       <c r="P11" s="4"/>
       <c r="Q11" s="5"/>
       <c r="R11" s="8"/>
-      <c r="S11" s="7"/>
-      <c r="T11" s="4"/>
-      <c r="U11" s="5"/>
-      <c r="V11" s="8"/>
-    </row>
-    <row r="12" spans="1:22" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:18" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>13</v>
       </c>
@@ -2061,17 +1914,13 @@
       <c r="R12" s="8">
         <v>5</v>
       </c>
-      <c r="S12" s="7"/>
-      <c r="T12" s="4"/>
-      <c r="U12" s="5"/>
-      <c r="V12" s="8"/>
-    </row>
-    <row r="13" spans="1:22" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:18" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>14</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C13" s="2">
         <v>5</v>
@@ -2107,17 +1956,13 @@
       <c r="R13" s="8">
         <v>1</v>
       </c>
-      <c r="S13" s="7"/>
-      <c r="T13" s="4"/>
-      <c r="U13" s="5"/>
-      <c r="V13" s="8"/>
-    </row>
-    <row r="14" spans="1:22" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:18" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C14" s="2">
         <v>2</v>
@@ -2167,17 +2012,13 @@
       <c r="R14" s="8">
         <v>5</v>
       </c>
-      <c r="S14" s="7"/>
-      <c r="T14" s="4"/>
-      <c r="U14" s="5"/>
-      <c r="V14" s="8"/>
-    </row>
-    <row r="15" spans="1:22" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:18" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C15" s="2">
         <v>5</v>
@@ -2205,17 +2046,13 @@
       <c r="R15" s="8">
         <v>5</v>
       </c>
-      <c r="S15" s="7"/>
-      <c r="T15" s="4"/>
-      <c r="U15" s="5"/>
-      <c r="V15" s="8"/>
-    </row>
-    <row r="16" spans="1:22" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:18" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C16" s="2">
         <v>5</v>
@@ -2249,17 +2086,13 @@
       <c r="P16" s="4"/>
       <c r="Q16" s="5"/>
       <c r="R16" s="8"/>
-      <c r="S16" s="7"/>
-      <c r="T16" s="4"/>
-      <c r="U16" s="5"/>
-      <c r="V16" s="8"/>
-    </row>
-    <row r="17" spans="1:22" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C17" s="2">
         <v>3</v>
@@ -2295,17 +2128,13 @@
       <c r="P17" s="4"/>
       <c r="Q17" s="5"/>
       <c r="R17" s="8"/>
-      <c r="S17" s="7"/>
-      <c r="T17" s="4"/>
-      <c r="U17" s="5"/>
-      <c r="V17" s="8"/>
-    </row>
-    <row r="18" spans="1:22" s="3" customFormat="1" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="32" t="s">
+    </row>
+    <row r="18" spans="1:18" s="3" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="33"/>
-      <c r="C18" s="34"/>
+      <c r="B18" s="48"/>
+      <c r="C18" s="49"/>
       <c r="D18" s="9">
         <f>SUMPRODUCT(C4:C17,D4:D17)</f>
         <v>188</v>
@@ -2366,241 +2195,198 @@
         <f>SUMPRODUCT(C4:C17,R4:R17)</f>
         <v>163</v>
       </c>
-      <c r="S18" s="13">
-        <f>SUMPRODUCT(C4:C17,S4:S17)</f>
-        <v>0</v>
-      </c>
-      <c r="T18" s="10">
-        <f>SUMPRODUCT(C4:C17,T4:T17)</f>
-        <v>0</v>
-      </c>
-      <c r="U18" s="11">
-        <f>SUMPRODUCT(C4:C17,U4:U17)</f>
-        <v>0</v>
-      </c>
-      <c r="V18" s="12">
-        <f>SUMPRODUCT(C4:C17,V4:V17)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:22" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="22"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="22"/>
-      <c r="J19" s="22"/>
-      <c r="K19" s="22"/>
-      <c r="L19" s="22"/>
-      <c r="M19" s="22"/>
-      <c r="N19" s="22"/>
-      <c r="O19" s="22"/>
-      <c r="P19" s="22"/>
-      <c r="Q19" s="22"/>
-      <c r="R19" s="22"/>
-      <c r="S19" s="22"/>
-      <c r="T19" s="22"/>
-      <c r="U19" s="22"/>
-      <c r="V19" s="22"/>
-    </row>
-    <row r="20" spans="1:22" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:18" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="37"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="37"/>
+      <c r="G19" s="37"/>
+      <c r="H19" s="37"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="37"/>
+      <c r="K19" s="37"/>
+      <c r="L19" s="37"/>
+      <c r="M19" s="37"/>
+      <c r="N19" s="37"/>
+      <c r="O19" s="37"/>
+      <c r="P19" s="37"/>
+      <c r="Q19" s="37"/>
+      <c r="R19" s="37"/>
+    </row>
+    <row r="20" spans="1:18" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="21"/>
       <c r="B20" s="21"/>
       <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
-      <c r="H20" s="38" t="s">
+      <c r="D20" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="I20" s="39"/>
-      <c r="J20" s="40"/>
-      <c r="K20" s="35" t="s">
+      <c r="E20" s="26"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="L20" s="36"/>
-      <c r="M20" s="36"/>
-      <c r="N20" s="37"/>
-      <c r="O20" s="38" t="s">
+      <c r="H20" s="23"/>
+      <c r="I20" s="23"/>
+      <c r="J20" s="24"/>
+      <c r="K20" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="P20" s="39"/>
-      <c r="Q20" s="40"/>
-      <c r="R20" s="15">
+      <c r="L20" s="26"/>
+      <c r="M20" s="27"/>
+      <c r="N20" s="15">
         <v>1</v>
       </c>
-      <c r="S20" s="35" t="s">
+      <c r="O20" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="T20" s="36"/>
-      <c r="U20" s="36"/>
-      <c r="V20" s="37"/>
-    </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="P20" s="35"/>
+      <c r="Q20" s="35"/>
+      <c r="R20" s="36"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="20"/>
       <c r="B21" s="20"/>
       <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
-      <c r="H21" s="41"/>
-      <c r="I21" s="42"/>
-      <c r="J21" s="43"/>
-      <c r="K21" s="35" t="s">
+      <c r="D21" s="28"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="L21" s="36"/>
-      <c r="M21" s="36"/>
-      <c r="N21" s="37"/>
-      <c r="O21" s="41"/>
-      <c r="P21" s="42"/>
-      <c r="Q21" s="43"/>
-      <c r="R21" s="15">
+      <c r="H21" s="23"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="24"/>
+      <c r="K21" s="28"/>
+      <c r="L21" s="29"/>
+      <c r="M21" s="30"/>
+      <c r="N21" s="15">
         <v>2</v>
       </c>
-      <c r="S21" s="35" t="s">
+      <c r="O21" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="T21" s="36"/>
-      <c r="U21" s="36"/>
-      <c r="V21" s="37"/>
-    </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="P21" s="35"/>
+      <c r="Q21" s="35"/>
+      <c r="R21" s="36"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="20"/>
       <c r="B22" s="20"/>
       <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
-      <c r="H22" s="41"/>
-      <c r="I22" s="42"/>
-      <c r="J22" s="43"/>
-      <c r="K22" s="35" t="s">
+      <c r="D22" s="28"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="30"/>
+      <c r="G22" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="L22" s="36"/>
-      <c r="M22" s="36"/>
-      <c r="N22" s="37"/>
-      <c r="O22" s="41"/>
-      <c r="P22" s="42"/>
-      <c r="Q22" s="43"/>
-      <c r="R22" s="15">
-        <v>3</v>
-      </c>
-      <c r="S22" s="35" t="s">
+      <c r="H22" s="23"/>
+      <c r="I22" s="23"/>
+      <c r="J22" s="24"/>
+      <c r="K22" s="28"/>
+      <c r="L22" s="29"/>
+      <c r="M22" s="30"/>
+      <c r="N22" s="15">
+        <v>3</v>
+      </c>
+      <c r="O22" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="T22" s="36"/>
-      <c r="U22" s="36"/>
-      <c r="V22" s="37"/>
-    </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="P22" s="35"/>
+      <c r="Q22" s="35"/>
+      <c r="R22" s="36"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="20"/>
       <c r="B23" s="20"/>
       <c r="C23" s="20"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="20"/>
-      <c r="H23" s="41"/>
-      <c r="I23" s="42"/>
-      <c r="J23" s="43"/>
-      <c r="K23" s="35" t="s">
+      <c r="D23" s="28"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="30"/>
+      <c r="G23" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="L23" s="36"/>
-      <c r="M23" s="36"/>
-      <c r="N23" s="37"/>
-      <c r="O23" s="41"/>
-      <c r="P23" s="42"/>
-      <c r="Q23" s="43"/>
-      <c r="R23" s="15">
+      <c r="H23" s="23"/>
+      <c r="I23" s="23"/>
+      <c r="J23" s="24"/>
+      <c r="K23" s="28"/>
+      <c r="L23" s="29"/>
+      <c r="M23" s="30"/>
+      <c r="N23" s="15">
         <v>4</v>
       </c>
-      <c r="S23" s="35" t="s">
+      <c r="O23" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="T23" s="36"/>
-      <c r="U23" s="36"/>
-      <c r="V23" s="37"/>
-    </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="P23" s="35"/>
+      <c r="Q23" s="35"/>
+      <c r="R23" s="36"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="20"/>
       <c r="B24" s="20"/>
       <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="H24" s="44"/>
-      <c r="I24" s="45"/>
-      <c r="J24" s="46"/>
-      <c r="K24" s="35" t="s">
+      <c r="D24" s="31"/>
+      <c r="E24" s="32"/>
+      <c r="F24" s="33"/>
+      <c r="G24" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="L24" s="36"/>
-      <c r="M24" s="36"/>
-      <c r="N24" s="37"/>
-      <c r="O24" s="44"/>
-      <c r="P24" s="45"/>
-      <c r="Q24" s="46"/>
-      <c r="R24" s="15">
-        <v>5</v>
-      </c>
-      <c r="S24" s="35" t="s">
+      <c r="H24" s="23"/>
+      <c r="I24" s="23"/>
+      <c r="J24" s="24"/>
+      <c r="K24" s="31"/>
+      <c r="L24" s="32"/>
+      <c r="M24" s="33"/>
+      <c r="N24" s="15">
+        <v>5</v>
+      </c>
+      <c r="O24" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="T24" s="36"/>
-      <c r="U24" s="36"/>
-      <c r="V24" s="37"/>
-    </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="P24" s="35"/>
+      <c r="Q24" s="35"/>
+      <c r="R24" s="36"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B25" s="3"/>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="14"/>
       <c r="F26" s="14"/>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="14"/>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="14"/>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="14"/>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="14"/>
     </row>
-    <row r="35" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J35" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="21">
-    <mergeCell ref="H20:J24"/>
-    <mergeCell ref="O20:Q24"/>
-    <mergeCell ref="K20:N20"/>
-    <mergeCell ref="K21:N21"/>
-    <mergeCell ref="K22:N22"/>
-    <mergeCell ref="K23:N23"/>
-    <mergeCell ref="K24:N24"/>
-    <mergeCell ref="S20:V20"/>
-    <mergeCell ref="S21:V21"/>
-    <mergeCell ref="S22:V22"/>
-    <mergeCell ref="S23:V23"/>
-    <mergeCell ref="S24:V24"/>
-    <mergeCell ref="A19:V19"/>
-    <mergeCell ref="A1:V1"/>
+  <mergeCells count="13">
+    <mergeCell ref="A19:R19"/>
+    <mergeCell ref="A1:R1"/>
     <mergeCell ref="D2:G2"/>
     <mergeCell ref="H2:J2"/>
     <mergeCell ref="K2:N2"/>
     <mergeCell ref="O2:R2"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A18:C18"/>
-    <mergeCell ref="S2:V2"/>
+    <mergeCell ref="O20:R20"/>
+    <mergeCell ref="O21:R21"/>
+    <mergeCell ref="O22:R22"/>
+    <mergeCell ref="O23:R23"/>
+    <mergeCell ref="O24:R24"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -2616,7 +2402,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Diagramms and some text for Conzepts
</commit_message>
<xml_diff>
--- a/Bewertungsmatrixnew.xlsx
+++ b/Bewertungsmatrixnew.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="26709"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/heuby/git/masterthesis/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2100" yWindow="6120" windowWidth="24765" windowHeight="16440"/>
+    <workbookView xWindow="19060" yWindow="4100" windowWidth="24760" windowHeight="16440"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -683,42 +688,42 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="24" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="14" xfId="4" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="15" xfId="4" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="16" xfId="4" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Currency" xfId="3" builtinId="4"/>
@@ -1341,7 +1346,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1352,68 +1357,68 @@
   <dimension ref="A1:R35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="X3" sqref="X3"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" customWidth="1"/>
-    <col min="2" max="2" width="45.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="18" width="4.42578125" customWidth="1"/>
+    <col min="1" max="1" width="6.33203125" customWidth="1"/>
+    <col min="2" max="2" width="45.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="18" width="4.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="38" t="s">
+    <row r="1" spans="1:18" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-      <c r="L1" s="38"/>
-      <c r="M1" s="38"/>
-      <c r="N1" s="38"/>
-      <c r="O1" s="38"/>
-      <c r="P1" s="38"/>
-      <c r="Q1" s="38"/>
-      <c r="R1" s="38"/>
-    </row>
-    <row r="2" spans="1:18" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="45"/>
-      <c r="B2" s="45"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="39" t="s">
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="35"/>
+      <c r="O1" s="35"/>
+      <c r="P1" s="35"/>
+      <c r="Q1" s="35"/>
+      <c r="R1" s="35"/>
+    </row>
+    <row r="2" spans="1:18" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="42"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="39" t="s">
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="39" t="s">
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40"/>
-      <c r="N2" s="41"/>
-      <c r="O2" s="42" t="s">
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="P2" s="43"/>
-      <c r="Q2" s="43"/>
-      <c r="R2" s="44"/>
-    </row>
-    <row r="3" spans="1:18" ht="132.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P2" s="40"/>
+      <c r="Q2" s="40"/>
+      <c r="R2" s="41"/>
+    </row>
+    <row r="3" spans="1:18" ht="133" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
@@ -1469,7 +1474,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>5</v>
       </c>
@@ -1519,7 +1524,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>6</v>
       </c>
@@ -1575,7 +1580,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>7</v>
       </c>
@@ -1609,7 +1614,7 @@
       <c r="Q6" s="5"/>
       <c r="R6" s="8"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>8</v>
       </c>
@@ -1665,7 +1670,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>9</v>
       </c>
@@ -1721,7 +1726,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>10</v>
       </c>
@@ -1777,7 +1782,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>11</v>
       </c>
@@ -1833,7 +1838,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>12</v>
       </c>
@@ -1859,7 +1864,7 @@
       <c r="Q11" s="5"/>
       <c r="R11" s="8"/>
     </row>
-    <row r="12" spans="1:18" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>13</v>
       </c>
@@ -1879,7 +1884,7 @@
         <v>3</v>
       </c>
       <c r="G12" s="8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H12" s="7">
         <v>5</v>
@@ -1915,7 +1920,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:18" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>14</v>
       </c>
@@ -1957,7 +1962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:18" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>15</v>
       </c>
@@ -2013,7 +2018,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:18" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>16</v>
       </c>
@@ -2047,7 +2052,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:18" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>58</v>
       </c>
@@ -2087,7 +2092,7 @@
       <c r="Q16" s="5"/>
       <c r="R16" s="8"/>
     </row>
-    <row r="17" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>60</v>
       </c>
@@ -2129,12 +2134,12 @@
       <c r="Q17" s="5"/>
       <c r="R17" s="8"/>
     </row>
-    <row r="18" spans="1:18" s="3" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="47" t="s">
+    <row r="18" spans="1:18" s="3" customFormat="1" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="48"/>
-      <c r="C18" s="49"/>
+      <c r="B18" s="45"/>
+      <c r="C18" s="46"/>
       <c r="D18" s="9">
         <f>SUMPRODUCT(C4:C17,D4:D17)</f>
         <v>188</v>
@@ -2149,7 +2154,7 @@
       </c>
       <c r="G18" s="12">
         <f>SUMPRODUCT(C4:C17,G4:G17)</f>
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="H18" s="13">
         <f>SUMPRODUCT(C4:C17,H4:H17)</f>
@@ -2196,27 +2201,27 @@
         <v>163</v>
       </c>
     </row>
-    <row r="19" spans="1:18" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="37"/>
-      <c r="B19" s="37"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="37"/>
-      <c r="G19" s="37"/>
-      <c r="H19" s="37"/>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
-      <c r="K19" s="37"/>
-      <c r="L19" s="37"/>
-      <c r="M19" s="37"/>
-      <c r="N19" s="37"/>
-      <c r="O19" s="37"/>
-      <c r="P19" s="37"/>
-      <c r="Q19" s="37"/>
-      <c r="R19" s="37"/>
-    </row>
-    <row r="20" spans="1:18" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="34"/>
+      <c r="B19" s="34"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="34"/>
+      <c r="E19" s="34"/>
+      <c r="F19" s="34"/>
+      <c r="G19" s="34"/>
+      <c r="H19" s="34"/>
+      <c r="I19" s="34"/>
+      <c r="J19" s="34"/>
+      <c r="K19" s="34"/>
+      <c r="L19" s="34"/>
+      <c r="M19" s="34"/>
+      <c r="N19" s="34"/>
+      <c r="O19" s="34"/>
+      <c r="P19" s="34"/>
+      <c r="Q19" s="34"/>
+      <c r="R19" s="34"/>
+    </row>
+    <row r="20" spans="1:18" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="21"/>
       <c r="B20" s="21"/>
       <c r="C20" s="21"/>
@@ -2239,14 +2244,14 @@
       <c r="N20" s="15">
         <v>1</v>
       </c>
-      <c r="O20" s="34" t="s">
+      <c r="O20" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="P20" s="35"/>
-      <c r="Q20" s="35"/>
-      <c r="R20" s="36"/>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P20" s="48"/>
+      <c r="Q20" s="48"/>
+      <c r="R20" s="49"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" s="20"/>
       <c r="B21" s="20"/>
       <c r="C21" s="20"/>
@@ -2265,14 +2270,14 @@
       <c r="N21" s="15">
         <v>2</v>
       </c>
-      <c r="O21" s="34" t="s">
+      <c r="O21" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="P21" s="35"/>
-      <c r="Q21" s="35"/>
-      <c r="R21" s="36"/>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P21" s="48"/>
+      <c r="Q21" s="48"/>
+      <c r="R21" s="49"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" s="20"/>
       <c r="B22" s="20"/>
       <c r="C22" s="20"/>
@@ -2291,14 +2296,14 @@
       <c r="N22" s="15">
         <v>3</v>
       </c>
-      <c r="O22" s="34" t="s">
+      <c r="O22" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="P22" s="35"/>
-      <c r="Q22" s="35"/>
-      <c r="R22" s="36"/>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P22" s="48"/>
+      <c r="Q22" s="48"/>
+      <c r="R22" s="49"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" s="20"/>
       <c r="B23" s="20"/>
       <c r="C23" s="20"/>
@@ -2317,14 +2322,14 @@
       <c r="N23" s="15">
         <v>4</v>
       </c>
-      <c r="O23" s="34" t="s">
+      <c r="O23" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="P23" s="35"/>
-      <c r="Q23" s="35"/>
-      <c r="R23" s="36"/>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P23" s="48"/>
+      <c r="Q23" s="48"/>
+      <c r="R23" s="49"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24" s="20"/>
       <c r="B24" s="20"/>
       <c r="C24" s="20"/>
@@ -2343,37 +2348,42 @@
       <c r="N24" s="15">
         <v>5</v>
       </c>
-      <c r="O24" s="34" t="s">
+      <c r="O24" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="P24" s="35"/>
-      <c r="Q24" s="35"/>
-      <c r="R24" s="36"/>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P24" s="48"/>
+      <c r="Q24" s="48"/>
+      <c r="R24" s="49"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B25" s="3"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" s="14"/>
       <c r="F26" s="14"/>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" s="14"/>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A28" s="14"/>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A29" s="14"/>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A30" s="14"/>
     </row>
-    <row r="35" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J35" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="O20:R20"/>
+    <mergeCell ref="O21:R21"/>
+    <mergeCell ref="O22:R22"/>
+    <mergeCell ref="O23:R23"/>
+    <mergeCell ref="O24:R24"/>
     <mergeCell ref="A19:R19"/>
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="D2:G2"/>
@@ -2382,11 +2392,6 @@
     <mergeCell ref="O2:R2"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A18:C18"/>
-    <mergeCell ref="O20:R20"/>
-    <mergeCell ref="O21:R21"/>
-    <mergeCell ref="O22:R22"/>
-    <mergeCell ref="O23:R23"/>
-    <mergeCell ref="O24:R24"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -2402,7 +2407,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>